<commit_message>
updated, don't know why it's not working
</commit_message>
<xml_diff>
--- a/Lin_Rohner_lab4/Data_lab4A_stiction torque/backup.xlsx
+++ b/Lin_Rohner_lab4/Data_lab4A_stiction torque/backup.xlsx
@@ -52,10 +52,34 @@
           <t>Untitled</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Untitled 1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Untitled 2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Untitled 3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>-0.003550</v>
+        <v>0.000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.000007</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.656128</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.656128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>